<commit_message>
Strip trailing commas from each line of Csv
(sadly explodes the default Git Diffs)
</commit_message>
<xml_diff>
--- a/like-py.xlsx
+++ b/like-py.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plavarre/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plavarre/Public/like-py-xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8C110E-0D75-8F4A-A374-98853D739A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02690407-3720-B440-9729-CB4C522385EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="9" xr2:uid="{995B5C66-FA72-074C-87BA-100299560140}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{995B5C66-FA72-074C-87BA-100299560140}"/>
   </bookViews>
   <sheets>
     <sheet name="0 Welcome" sheetId="13" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="503">
   <si>
     <t>bit</t>
   </si>
@@ -1312,9 +1312,6 @@
   </si>
   <si>
     <t>## 8 Contributors</t>
-  </si>
-  <si>
-    <t>Thanks to my friends encouraging me to share our "like-py.xlsx" with you</t>
   </si>
   <si>
     <t>1 Welcome</t>
@@ -1371,9 +1368,6 @@
   </si>
   <si>
     <t>with a Search that finds</t>
-  </si>
-  <si>
-    <t>the LAMBDA and LET functions explained (poorly) inside</t>
   </si>
   <si>
     <t>to launch the Microsoft AutoUpdate app, and then</t>
@@ -1553,12 +1547,6 @@
     </r>
   </si>
   <si>
-    <t>You no longer have to type your code all out over again</t>
-  </si>
-  <si>
-    <t>as often you need your code to come work with you again,</t>
-  </si>
-  <si>
     <t>Excel &gt; Tab Formulas &gt; Define Name</t>
   </si>
   <si>
@@ -1574,9 +1562,6 @@
     <t>=LAMBDA(chars,
     LEFT(chars,FIND(" ",chars))
 )</t>
-  </si>
-  <si>
-    <t>Name it and call it</t>
   </si>
   <si>
     <t>=str.word("Hello Xlsx Like Py")</t>
@@ -1643,9 +1628,6 @@
     <t>These are our early days, not much here yet</t>
   </si>
   <si>
-    <t xml:space="preserve"> If you look for something difficult, you won't find here</t>
-  </si>
-  <si>
     <t>If you surprise this code with new test cases, it will betray you today</t>
   </si>
   <si>
@@ -1656,9 +1638,6 @@
   </si>
   <si>
     <t>for speaking the lyric line "do you love me like that",</t>
-  </si>
-  <si>
-    <t>such that I misheard the line as "do you love me like Pie?", which is a line I like lots : -)</t>
   </si>
   <si>
     <t>TL;DR: Call Python from inside Msft Beta Channel Office 365 Excel - Small Quick Xlsx Download - All Source No Binary</t>
@@ -1693,9 +1672,6 @@
   </si>
   <si>
     <t>1.4 Me personally,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I launched "pelavarre/like-py-xlsx" when they sold me </t>
   </si>
   <si>
     <t># We raise CalcError, where Excel raises ValueError, to reject negative lengths</t>
@@ -1999,6 +1975,33 @@
             IFERROR(MID(chars, last, LEN(sep)), ""),
             IFERROR(MID(chars, last + LEN(sep), LEN(chars)), "")
 )))</t>
+  </si>
+  <si>
+    <t>the LAMBDA and LET functions explained poorly inside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I launched "pelavarre/like-py-xlsx" back when they sold me </t>
+  </si>
+  <si>
+    <t>You no longer have to type your code all out over again,</t>
+  </si>
+  <si>
+    <t>as often you need your own code to come work with you again,</t>
+  </si>
+  <si>
+    <t>You can name it and you can call it by name</t>
+  </si>
+  <si>
+    <t>(or has Microsoft even opened up web spaces somewhere, as welcoming as Google Sheets?)</t>
+  </si>
+  <si>
+    <t>If you look for something difficult, you won't find here</t>
+  </si>
+  <si>
+    <t>Thanks to my friends for encouraging me to share our "like-py.xlsx" with you</t>
+  </si>
+  <si>
+    <t>such that I misheard this line as "do you love me like Pie?", which is a line I like lots : -)</t>
   </si>
 </sst>
 </file>
@@ -2597,9 +2600,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517CFC20-DDAA-7A41-A85E-ED9D5B318B48}">
-  <dimension ref="B3:G164"/>
+  <dimension ref="B3:G165"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2621,7 +2624,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
@@ -2631,43 +2634,43 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G11" s="36"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G12" s="36"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G13" s="36"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G14" s="36"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G15" s="36"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G16" s="36"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G17" s="36"/>
     </row>
@@ -2677,7 +2680,7 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
@@ -2687,84 +2690,84 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D28" s="35" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D31" s="35" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
-        <v>359</v>
+        <v>494</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D36" s="1"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D39" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D40" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D41" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D42" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D43" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C45" s="1" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.2">
@@ -2772,37 +2775,37 @@
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D47" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D48" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C53" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C57" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D57" s="10"/>
     </row>
@@ -2812,7 +2815,7 @@
     </row>
     <row r="59" spans="2:5" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E59" s="38" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="60" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2829,7 +2832,7 @@
     </row>
     <row r="62" spans="2:5" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E62" s="38" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="63" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2853,27 +2856,27 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="72" spans="2:5" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E72" s="38" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="73" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2888,22 +2891,22 @@
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B76" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="81" spans="3:5" ht="85" x14ac:dyDescent="0.2">
       <c r="E81" s="38" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
     </row>
     <row r="82" spans="3:5" x14ac:dyDescent="0.2">
@@ -2921,24 +2924,24 @@
     </row>
     <row r="84" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="85" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C85" s="36" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D85" s="36"/>
     </row>
     <row r="86" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C86" s="36" t="s">
-        <v>385</v>
+        <v>496</v>
       </c>
       <c r="D86" s="36"/>
     </row>
     <row r="87" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C87" s="36" t="s">
-        <v>386</v>
+        <v>497</v>
       </c>
       <c r="D87" s="36"/>
     </row>
@@ -2948,7 +2951,7 @@
     </row>
     <row r="89" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D89" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="90" spans="3:5" x14ac:dyDescent="0.2">
@@ -2958,32 +2961,32 @@
     </row>
     <row r="91" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D91" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="93" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E93" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="95" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D95" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="97" spans="2:5" ht="51" x14ac:dyDescent="0.2">
       <c r="E97" s="38" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C99" t="s">
-        <v>392</v>
+        <v>498</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E101" s="27" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.2">
@@ -2994,22 +2997,22 @@
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C104" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D106" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D107" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D108" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.2">
@@ -3024,12 +3027,12 @@
     </row>
     <row r="115" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C115" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="116" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C116" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="118" spans="3:5" x14ac:dyDescent="0.2">
@@ -3037,138 +3040,143 @@
         <v>338</v>
       </c>
     </row>
-    <row r="120" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C120" t="s">
-        <v>400</v>
+    <row r="119" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C119" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="121" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C121" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="123" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C123" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="125" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E125" s="27" t="s">
-        <v>404</v>
+        <v>395</v>
+      </c>
+    </row>
+    <row r="122" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C122" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="124" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C124" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="126" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E126" t="str" cm="1">
-        <f t="array" ref="E126">list.item(str.rpartition("C:\My Documents\like-py.xlsx", "\"), -1)</f>
+      <c r="E126" s="27" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="127" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E127" t="str" cm="1">
+        <f t="array" ref="E127">list.item(str.rpartition("C:\My Documents\like-py.xlsx", "\"), -1)</f>
         <v>C:\My Documents</v>
       </c>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B129" t="s">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B130" t="s">
         <v>339</v>
-      </c>
-    </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C131" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C132" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C134" s="35" t="s">
-        <v>408</v>
+        <v>401</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C133" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C135" s="35"/>
+      <c r="C135" s="35" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D136" t="s">
-        <v>409</v>
-      </c>
+      <c r="C136" s="35"/>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D137" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D138" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B141" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D139" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B142" s="1" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C143" t="s">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C144" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C145" t="s">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C146" t="s">
         <v>341</v>
-      </c>
-    </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C147" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C148" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C149" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C151" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C153" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C150" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C152" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C154" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C155" t="s">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C156" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B158" s="1" t="s">
+    <row r="159" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B159" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C160" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="162" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C162" t="s">
-        <v>416</v>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C161" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C163" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
     </row>
     <row r="164" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C164" t="s">
-        <v>418</v>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C165" t="s">
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -3184,7 +3192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D852BB-57DF-6140-815D-350948B01B5D}">
   <dimension ref="B3:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -4272,22 +4280,22 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="15" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="21" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -4321,7 +4329,7 @@
         <v>False</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
@@ -4334,7 +4342,7 @@
         <v>True</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
@@ -4368,7 +4376,7 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="10" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
@@ -4534,7 +4542,7 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
@@ -4542,17 +4550,17 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="21" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -4563,7 +4571,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E10" s="1" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -4571,10 +4579,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -4586,7 +4594,7 @@
         <v>-123</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
@@ -4598,7 +4606,7 @@
         <v>-1</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
@@ -4640,7 +4648,7 @@
         <v>123.456</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
@@ -4714,7 +4722,7 @@
         <v>0b1111111111</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
@@ -4808,7 +4816,7 @@
         <v>9</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
@@ -4884,7 +4892,7 @@
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C48" s="22"/>
       <c r="E48" s="1" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -4892,10 +4900,10 @@
         <v>23</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
@@ -4907,7 +4915,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
@@ -4977,10 +4985,10 @@
         <v>23</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
@@ -4992,12 +5000,12 @@
         <v>0</v>
       </c>
       <c r="E64" s="22" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E65" s="22" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
@@ -5070,7 +5078,7 @@
         <v>0xFFFFFFFFFF</v>
       </c>
       <c r="E75" s="22" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
@@ -5208,7 +5216,7 @@
         <v>0x7777777777</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.2">
@@ -5342,7 +5350,7 @@
         <v>0</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.2">
@@ -5366,7 +5374,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="E113" s="10" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.2">
@@ -5378,7 +5386,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="E114" s="10" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
     </row>
     <row r="117" spans="2:5" x14ac:dyDescent="0.2">
@@ -5464,7 +5472,7 @@
         <v>-0.4</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.2">
@@ -5558,7 +5566,7 @@
         <v>0.5</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.2">
@@ -5579,7 +5587,7 @@
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E152" s="1" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
     </row>
     <row r="153" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -5587,10 +5595,10 @@
         <v>40</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.2">
@@ -5604,12 +5612,12 @@
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E157" s="1" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="158" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="E158" s="2" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="159" spans="2:5" x14ac:dyDescent="0.2">
@@ -5617,7 +5625,7 @@
         <v>40</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
     </row>
     <row r="160" spans="2:5" x14ac:dyDescent="0.2">
@@ -5631,17 +5639,17 @@
     </row>
     <row r="163" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E163" s="1" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
     </row>
     <row r="164" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E164" s="10" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
     </row>
     <row r="165" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E165" s="10" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -5667,22 +5675,22 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -5716,7 +5724,7 @@
         <v>89</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
@@ -5728,7 +5736,7 @@
         <v>-123.0</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -5740,7 +5748,7 @@
         <v>-1.23</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
@@ -5845,7 +5853,7 @@
         <v>42</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -5857,7 +5865,7 @@
         <v>-1</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -5869,7 +5877,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
@@ -5894,7 +5902,7 @@
         <v>92</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
@@ -5913,7 +5921,7 @@
     </row>
     <row r="45" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="E45" s="2" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
@@ -5956,17 +5964,17 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B1" s="8" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
@@ -6003,7 +6011,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -6015,7 +6023,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
@@ -6047,7 +6055,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -6148,7 +6156,7 @@
         <v>29</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
@@ -6172,7 +6180,7 @@
         <v>29</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
@@ -6199,7 +6207,7 @@
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E38" s="3" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
@@ -6211,7 +6219,7 @@
         <v/>
       </c>
       <c r="E39" s="3" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
@@ -6271,7 +6279,7 @@
         <v>ab'cd</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
@@ -6295,7 +6303,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
@@ -6386,7 +6394,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
@@ -6398,7 +6406,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
@@ -6407,24 +6415,24 @@
         <v>#NUM!</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E63" s="10" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="E64" s="10" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E65" s="3" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
@@ -6494,7 +6502,7 @@
         <v>15</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.2">
@@ -6547,7 +6555,7 @@
         <v>512</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.2">
@@ -6563,7 +6571,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.2">
@@ -6572,7 +6580,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.2">
@@ -6582,7 +6590,7 @@
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E93" s="10" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.2">
@@ -6592,7 +6600,7 @@
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E96" s="10" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.2">
@@ -6602,12 +6610,12 @@
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E99" s="10" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B101" s="15" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>156</v>
@@ -6626,18 +6634,18 @@
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B105" s="15" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="C105" s="10"/>
       <c r="E105" s="1" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B106" s="10"/>
       <c r="C106" s="10"/>
       <c r="E106" s="22" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.2">
@@ -6707,7 +6715,7 @@
     </row>
     <row r="119" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B119" s="15" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>289</v>
@@ -6728,7 +6736,7 @@
     </row>
     <row r="123" spans="2:5" ht="192" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E123" s="2" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="124" spans="2:5" x14ac:dyDescent="0.2">
@@ -6875,7 +6883,7 @@
     </row>
     <row r="148" spans="2:5" ht="208" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E148" s="2" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.2">
@@ -6937,7 +6945,7 @@
     </row>
     <row r="167" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E167" s="10" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -7432,14 +7440,14 @@
       <c r="B76" s="11"/>
       <c r="C76" s="13"/>
       <c r="E76" s="4" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="77" spans="2:5" ht="85" x14ac:dyDescent="0.2">
       <c r="B77" s="11"/>
       <c r="C77" s="13"/>
       <c r="E77" s="6" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.2">
@@ -8211,7 +8219,7 @@
       </c>
       <c r="D103" s="3"/>
       <c r="E103" s="5" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.2">
@@ -8467,7 +8475,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
@@ -8596,7 +8604,7 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Settle on 'kwarg_eq_value' style, to decipher calling with Bool
Also add a Makefile, to make pushing Xlsx changes quicker
Also demo the open puzzle at _repr of List of Str
Also empty the trash can at Scraps Csv
</commit_message>
<xml_diff>
--- a/like-py.xlsx
+++ b/like-py.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10627"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plavarre/Public/like-py-xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F3E1FC-6508-964C-801A-EB2984F59D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2B9A86-7E14-1E4B-9DF5-74CC921A8AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{995B5C66-FA72-074C-87BA-100299560140}"/>
   </bookViews>
@@ -63,13 +63,13 @@
     <definedName name="str.any">_xlfn.LAMBDA(_xlpm.chars, IF(LEN(_xlpm.chars), TRUE))</definedName>
     <definedName name="str.bool">_xlfn.LAMBDA(_xlpm.chars, IF(LEN(_xlpm.chars), TRUE))</definedName>
     <definedName name="str.endswith">_xlfn.LAMBDA(_xlpm.chars,_xlpm.suffix,      IF(LEN(_xlpm.suffix) &lt;= LEN(_xlpm.chars),          MID(_xlpm.chars, LEN(_xlpm.chars) - LEN(_xlpm.suffix) + 1, LEN(_xlpm.suffix)) = _xlpm.suffix,          FALSE))</definedName>
-    <definedName name="str.eval">_xlfn.LAMBDA(_xlpm.chars,      _xlfn.LET(          _xlpm.body, MID(_xlpm.chars, 2, LEN(_xlpm.chars) - 2),          _xlpm.stops, _xlfn.SEQUENCE(MAX(1, LEN(_xlpm.body))),          _xlpm.picks, MID(_xlpm.body, _xlpm.stops, 1),          _xlpm.pairs, MID(_xlpm.body, _xlpm.stops, 2),          _xlpm.cuts, IF(_xlpm.picks = "\", "", _xlpm.picks),          _xlpm.patches, IF(_xlpm.pairs = "\\", "\", _xlpm.cuts),          _xlpm.ignore_empty, TRUE,          _xlpm.joined, _xlfn.TEXTJOIN("", _xlpm.ignore_empty, _xlpm.patches),          _xlpm.joined  ))</definedName>
+    <definedName name="str.eval">_xlfn.LAMBDA(_xlpm.chars,      _xlfn.LET(          _xlpm.body, MID(_xlpm.chars, 2, LEN(_xlpm.chars) - 2),          _xlpm.stops, _xlfn.SEQUENCE(MAX(1, LEN(_xlpm.body))),          _xlpm.picks, MID(_xlpm.body, _xlpm.stops, 1),          _xlpm.pairs, MID(_xlpm.body, _xlpm.stops, 2),          _xlpm.cuts, IF(_xlpm.picks = "\", "", _xlpm.picks),          _xlpm.patches, IF(_xlpm.pairs = "\\", "\", _xlpm.cuts),          _xlpm.ignore_empty_eq_true, TRUE,          _xlpm.joined, _xlfn.TEXTJOIN("", _xlpm.ignore_empty_eq_true, _xlpm.patches),          _xlpm.joined  ))</definedName>
     <definedName name="str.int">_xlfn.LAMBDA(_xlpm.chars,      _xlfn.IFS(          LEN(_xlpm.chars) = 0,              #NUM!,          LEFT(_xlpm.chars, 1) = "+",              _xlfn.DECIMAL(MID(_xlpm.chars, 2, LEN(_xlpm.chars)), 10),          LEFT(_xlpm.chars, 1) = "-",              -_xlfn.DECIMAL(MID(_xlpm.chars, 2, LEN(_xlpm.chars)), 10),          TRUE,              _xlfn.DECIMAL(_xlpm.chars, 10)  ))</definedName>
     <definedName name="str.int_base">_xlfn.LAMBDA(_xlpm.chars,_xlpm.base,      _xlfn.LET(          _xlpm.ch, LEFT(_xlpm.chars, 1),          _xlpm.signed, IF(_xlpm.ch = "-", TRUE, IF(_xlpm.ch = "+", TRUE)),          _xlpm.digits, IF(_xlpm.signed,              MID(_xlpm.chars, 2, LEN(_xlpm.chars)),              _xlpm.chars),          _xlpm.eval1, IF(_xlpm.base &lt;&gt; 0,              _xlfn.DECIMAL(_xlpm.digits, _xlpm.base),              _xlfn.LET(                  _xlpm.lows, LOWER(_xlpm.digits),                  _xlfn.IFS(                      MID(_xlpm.lows, 1, 2) = "0b",                          BIN2DEC(MID(_xlpm.digits, 3, LEN(_xlpm.digits))),                      MID(_xlpm.lows, 1, 2) = "0o",                          OCT2DEC(MID(_xlpm.digits, 3, LEN(_xlpm.digits))),                      MID(_xlpm.lows, 1, 2) = "0x",                          HEX2DEC(MID(_xlpm.digits, 3, LEN(_xlpm.digits))),                      TRUE,                          _xlfn.DECIMAL(_xlpm.digits, 10)              ))),          _xlpm.sign, IF(_xlpm.ch = "-", -1, 1),          _xlpm.eval2, _xlpm.sign * _xlpm.eval1,          _xlpm.eval2  ))</definedName>
     <definedName name="str.int_base_2">_xlfn.LAMBDA(_xlpm.chars,      _xlfn.LET(          _xlpm.head, LEFT(_xlpm.chars, 1),          _xlpm.signed, OR(_xlpm.head = "-", _xlpm.head = "+"),          _xlpm.unsigned, RIGHT(_xlpm.chars, LEN(_xlpm.chars) - 1),          _xlpm.tail, IF(_xlpm.signed, _xlpm.unsigned, _xlpm.chars),          _xlpm.based, LEFT(_xlpm.tail, 2) = "0b",          _xlpm.unbased, RIGHT(_xlpm.tail, LEN(_xlpm.tail) - 2),          _xlpm.digits, IF(_xlpm.based, _xlpm.unbased, _xlpm.tail),          _xlpm.sign, IF(_xlpm.head = "-", -1, 1),          _xlpm.base, IF(_xlpm.head = "", 0, 2),          _xlpm.evalled, _xlpm.sign * _xlfn.DECIMAL(_xlpm.digits, _xlpm.base),          _xlpm.evalled  ))</definedName>
     <definedName name="str.ord">_xlfn.LAMBDA(_xlpm.chars, _xlfn.UNICODE(_xlpm.chars))</definedName>
     <definedName name="str.partition">_xlfn.LAMBDA(_xlpm.chars,_xlpm.sep,      _xlfn.LET(          _xlpm.stops, _xlfn.SEQUENCE(MAX(1, LEN(_xlpm.chars))),          _xlpm.picks, MID(_xlpm.chars, _xlpm.stops, LEN(_xlpm.sep)),          _xlpm.exact, 0,          _xlpm.last, _xlfn.XMATCH(TRUE, _xlpm.picks = _xlpm.sep, _xlpm.exact),          CHOOSE(              {1;2;3},              IFERROR(MID(_xlpm.chars, 1, _xlpm.last - 1), _xlpm.chars),              IFERROR(MID(_xlpm.chars, _xlpm.last, LEN(_xlpm.sep)), ""),              IFERROR(MID(_xlpm.chars, _xlpm.last + LEN(_xlpm.sep), LEN(_xlpm.chars)), "")  )))</definedName>
-    <definedName name="str.repr">_xlfn.LAMBDA(_xlpm.chars,      _xlfn.LET(          _xlpm.stops, _xlfn.SEQUENCE(MAX(1, LEN(_xlpm.chars))),          _xlpm.picks, MID(_xlpm.chars, _xlpm.stops, 1),          _xlpm.slashes, IF(_xlpm.picks = "\", "\\", _xlpm.picks),          _xlpm.ticks, IF(_xlpm.picks = "'", "\'", _xlpm.slashes),          _xlpm.doubles, IF(_xlpm.picks = """", "\""", _xlpm.ticks),          _xlpm.ignore_empty, TRUE,          _xlpm.joined, _xlfn.TEXTJOIN("", _xlpm.ignore_empty, _xlpm.doubles),          _xlpm.quoted, "'" &amp; _xlpm.joined &amp; "'",          _xlpm.quoted  ))</definedName>
+    <definedName name="str.repr">_xlfn.LAMBDA(_xlpm.chars,      _xlfn.LET(          _xlpm.stops, _xlfn.SEQUENCE(MAX(1, LEN(_xlpm.chars))),          _xlpm.picks, MID(_xlpm.chars, _xlpm.stops, 1),          _xlpm.slashes, IF(_xlpm.picks = "\", "\\", _xlpm.picks),          _xlpm.ticks, IF(_xlpm.picks = "'", "\'", _xlpm.slashes),          _xlpm.doubles, IF(_xlpm.picks = """", "\""", _xlpm.ticks),          _xlpm.ignore_empty_eq_true, TRUE,          _xlpm.joined, _xlfn.TEXTJOIN("", _xlpm.ignore_empty_eq_true, _xlpm.doubles),          _xlpm.quoted, "'" &amp; _xlpm.joined &amp; "'",          _xlpm.quoted  ))</definedName>
     <definedName name="str.rpartition">_xlfn.LAMBDA(_xlpm.chars,_xlpm.sep,      _xlfn.LET(          _xlpm.stops, _xlfn.SEQUENCE(MAX(1, LEN(_xlpm.chars))),          _xlpm.picks, MID(_xlpm.chars, _xlpm.stops, LEN(_xlpm.sep)),          _xlpm.exact, 0,          _xlpm.reverse, -1,          _xlpm.last, _xlfn.XMATCH(TRUE, _xlpm.picks = _xlpm.sep, _xlpm.exact, _xlpm.reverse),          CHOOSE(              {1;2;3},              IFERROR(MID(_xlpm.chars, 1, _xlpm.last - 1), _xlpm.chars),              IFERROR(MID(_xlpm.chars, _xlpm.last, LEN(_xlpm.sep)), ""),              IFERROR(MID(_xlpm.chars, _xlpm.last + LEN(_xlpm.sep), LEN(_xlpm.chars)), "")  )))</definedName>
     <definedName name="str.word">_xlfn.LAMBDA(_xlpm.chars,      LEFT(_xlpm.chars, FIND(" ",_xlpm.chars) - 1)  )</definedName>
   </definedNames>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="515">
   <si>
     <t>bit</t>
   </si>
@@ -544,16 +544,6 @@
   </si>
   <si>
     <t>def list.repr(items)</t>
-  </si>
-  <si>
-    <t>=LAMBDA(items,
-    LET(
-        ignore_empty, FALSE,
-        "[" &amp; TEXTJOIN(
-            ", ",
-            ignore_empty,
-            items) &amp; "]"
-))</t>
   </si>
   <si>
     <t>list.repr(items)</t>
@@ -685,20 +675,6 @@
   </si>
   <si>
     <t>switch on basehint past + -: 0b 0o 0x else str.int</t>
-  </si>
-  <si>
-    <t>=LAMBDA(chars,
-    LET(
-        body, MID(chars, 2, LEN(chars) - 2),
-        stops, SEQUENCE(MAX(1, LEN(body))),
-        picks, MID(body, stops, 1),
-        pairs, MID(body, stops, 2),
-        cuts, IF(picks = "\", "", picks),
-        patches, IF(pairs = "\\", "\", cuts),
-        ignore_empty, TRUE,
-        joined, TEXTJOIN("", ignore_empty, patches),
-        joined
-))("'abc\\def\""ghi\'kjl'")</t>
   </si>
   <si>
     <t>=LAMBDA(chars,
@@ -720,20 +696,6 @@
     <t>="0b10"&amp;"0000"&amp;"0000"</t>
   </si>
   <si>
-    <t>=LAMBDA(chars,
-    LET(
-        stops, SEQUENCE(MAX(1, LEN(chars))),
-        picks, MID(chars, stops, 1),
-        slashes, IF(picks = "\", "\\", picks),
-        ticks, IF(picks = "'", "\'", slashes),
-        doubles, IF(picks = """", "\""", ticks),
-        ignore_empty, TRUE,
-        joined, TEXTJOIN("", ignore_empty, doubles),
-        quoted, "'" &amp; joined &amp; "'",
-        quoted
-))</t>
-  </si>
-  <si>
     <t># Python "repr" encloses even single quotes in single quotes</t>
   </si>
   <si>
@@ -846,24 +808,6 @@
     <t>def str.endswith(chars, suffix)</t>
   </si>
   <si>
-    <t>def bool.as_integer_ratio(bit)</t>
-  </si>
-  <si>
-    <t>=LAMBDA(bit, IF(bit, {1;1}, {0;1}))</t>
-  </si>
-  <si>
-    <t>bool.as_integer_ratio(bit)</t>
-  </si>
-  <si>
-    <t>def bool.bit_length(bit)</t>
-  </si>
-  <si>
-    <t># same code for def bool.bit_length/ .float/ .int</t>
-  </si>
-  <si>
-    <t>bool.bit_length(bit)</t>
-  </si>
-  <si>
     <t>str.endswith(
 chars, suffix
 )</t>
@@ -897,9 +841,6 @@
   </si>
   <si>
     <t>int.bit_length(i)</t>
-  </si>
-  <si>
-    <t>=LAMBDA(I, INT(IF(i, LOG(ABS(i), 2) + 1)))</t>
   </si>
   <si>
     <t>=LAMBDA(i, INT(IF(i, LOG(ABS(i), 2) + 1)))</t>
@@ -2073,6 +2014,56 @@
   </si>
   <si>
     <t>Collect Trash</t>
+  </si>
+  <si>
+    <t>=LAMBDA(chars,
+    LET(
+        body, MID(chars, 2, LEN(chars) - 2),
+        stops, SEQUENCE(MAX(1, LEN(body))),
+        picks, MID(body, stops, 1),
+        pairs, MID(body, stops, 2),
+        cuts, IF(picks = "\", "", picks),
+        patches, IF(pairs = "\\", "\", cuts),
+        ignore_empty_eq_true, TRUE,
+        joined, TEXTJOIN("", ignore_empty_eq_true, patches),
+        joined
+))("'abc\\def\""ghi\'kjl'")</t>
+  </si>
+  <si>
+    <t>=LAMBDA(chars,
+    LET(
+        stops, SEQUENCE(MAX(1, LEN(chars))),
+        picks, MID(chars, stops, 1),
+        slashes, IF(picks = "\", "\\", picks),
+        ticks, IF(picks = "'", "\'", slashes),
+        doubles, IF(picks = """", "\""", ticks),
+        ignore_empty_eq_true, TRUE,
+        joined, TEXTJOIN("", ignore_empty_eq_true, doubles),
+        quoted, "'" &amp; joined &amp; "'",
+        quoted
+))</t>
+  </si>
+  <si>
+    <t>=LAMBDA(items,
+    LET(
+        ignore_empty_eq_false, FALSE,
+        "[" &amp; TEXTJOIN(
+            ", ",
+            ignore_empty_eq_false,
+            items) &amp; "]"
+))</t>
+  </si>
+  <si>
+    <t>=CHOOSE({1;2;3},"aa","bb","cc")</t>
+  </si>
+  <si>
+    <t>str.repr(items)</t>
+  </si>
+  <si>
+    <t># TODO: wrong answer</t>
+  </si>
+  <si>
+    <t># TODO: #N/A is a fair answer here, but can we solve list.repr?</t>
   </si>
 </sst>
 </file>
@@ -2682,12 +2673,12 @@
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="37" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
@@ -2695,53 +2686,53 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="G11" s="36"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="G12" s="36"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="G13" s="36"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="G14" s="36"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="G15" s="36"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="G16" s="36"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="G17" s="36"/>
     </row>
@@ -2751,94 +2742,94 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D28" s="35" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D31" s="35" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="D36" s="1"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D39" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D40" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D41" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D42" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D43" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C45" s="1" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.2">
@@ -2846,37 +2837,37 @@
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D47" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D48" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C53" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C57" s="10" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="D57" s="10"/>
     </row>
@@ -2886,7 +2877,7 @@
     </row>
     <row r="59" spans="2:5" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E59" s="38" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
     </row>
     <row r="60" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2903,7 +2894,7 @@
     </row>
     <row r="62" spans="2:5" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E62" s="38" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
     </row>
     <row r="63" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2927,27 +2918,27 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="72" spans="2:5" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E72" s="38" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
     </row>
     <row r="73" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2962,22 +2953,22 @@
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B76" s="1" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
     </row>
     <row r="81" spans="3:5" ht="85" x14ac:dyDescent="0.2">
       <c r="E81" s="38" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
     </row>
     <row r="82" spans="3:5" x14ac:dyDescent="0.2">
@@ -2995,24 +2986,24 @@
     </row>
     <row r="84" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
     </row>
     <row r="85" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C85" s="36" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="D85" s="36"/>
     </row>
     <row r="86" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C86" s="36" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="D86" s="36"/>
     </row>
     <row r="87" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C87" s="36" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="D87" s="36"/>
     </row>
@@ -3022,37 +3013,37 @@
     </row>
     <row r="89" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D89" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
     </row>
     <row r="91" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D91" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
     </row>
     <row r="93" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E93" s="1" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
     </row>
     <row r="95" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D95" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
     </row>
     <row r="97" spans="2:5" ht="51" x14ac:dyDescent="0.2">
       <c r="E97" s="38" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C99" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E101" s="27" t="s">
-        <v>488</v>
+        <v>478</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.2">
@@ -3063,72 +3054,72 @@
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C104" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D106" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D107" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D108" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B111" s="1" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="113" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C113" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
     </row>
     <row r="115" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C115" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
     </row>
     <row r="116" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C116" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
     </row>
     <row r="118" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C118" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
     </row>
     <row r="119" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C119" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
     </row>
     <row r="121" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C121" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
     </row>
     <row r="122" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C122" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
     </row>
     <row r="124" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C124" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
     </row>
     <row r="126" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E126" s="27" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
     </row>
     <row r="127" spans="3:5" x14ac:dyDescent="0.2">
@@ -3139,22 +3130,22 @@
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C132" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C133" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C135" s="35" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.2">
@@ -3162,87 +3153,87 @@
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D137" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D138" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D139" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B142" s="1" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C144" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C146" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C148" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C149" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C150" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C152" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C154" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C156" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B159" s="1" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C161" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C163" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
     <row r="164" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C164" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C165" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -3256,1079 +3247,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D852BB-57DF-6140-815D-350948B01B5D}">
-  <dimension ref="B3:E76"/>
+  <dimension ref="B3"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="22" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="22"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="15" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="16" cm="1">
-        <f t="array" ref="C10:C11">bool.as_integer_ratio(B10)</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="15"/>
-      <c r="C11" s="16">
-        <v>1</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="15" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="C13" s="16" cm="1">
-        <f t="array" ref="C13:C14">bool.as_integer_ratio(B13)</f>
-        <v>1</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="15"/>
-      <c r="C14" s="16">
-        <v>1</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="B18" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="15" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="C19" s="13" cm="1">
-        <f t="array" ref="C19">bool.bit_length(B19)</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="15" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="C20" s="13" cm="1">
-        <f t="array" ref="C20">bool.bit_length(B20)</f>
-        <v>1</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="10">
-        <v>0</v>
-      </c>
-      <c r="C26" s="10">
-        <f t="shared" ref="C26:C57" si="0">2^B26-1</f>
-        <v>0</v>
-      </c>
-      <c r="D26" s="22" cm="1">
-        <f t="array" ref="D26">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C26)</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="10" t="b">
-        <f t="shared" ref="E26:E57" si="1">D26=B26</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="10">
-        <f t="shared" ref="B27:B58" si="2">B26+1</f>
-        <v>1</v>
-      </c>
-      <c r="C27" s="10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D27" s="22" cm="1">
-        <f t="array" ref="D27">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C27)</f>
-        <v>1</v>
-      </c>
-      <c r="E27" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="10">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="C28" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D28" s="22" cm="1">
-        <f t="array" ref="D28">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C28)</f>
-        <v>2</v>
-      </c>
-      <c r="E28" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="10">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="C29" s="10">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D29" s="22" cm="1">
-        <f t="array" ref="D29">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C29)</f>
-        <v>3</v>
-      </c>
-      <c r="E29" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="10">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="C30" s="10">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D30" s="22" cm="1">
-        <f t="array" ref="D30">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C30)</f>
-        <v>4</v>
-      </c>
-      <c r="E30" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="10">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="C31" s="10">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="D31" s="22" cm="1">
-        <f t="array" ref="D31">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C31)</f>
-        <v>5</v>
-      </c>
-      <c r="E31" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B32" s="10">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="C32" s="10">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="D32" s="22" cm="1">
-        <f t="array" ref="D32">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C32)</f>
-        <v>6</v>
-      </c>
-      <c r="E32" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="10">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="C33" s="10">
-        <f t="shared" si="0"/>
-        <v>127</v>
-      </c>
-      <c r="D33" s="22" cm="1">
-        <f t="array" ref="D33">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C33)</f>
-        <v>7</v>
-      </c>
-      <c r="E33" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="10">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="C34" s="10">
-        <f t="shared" si="0"/>
-        <v>255</v>
-      </c>
-      <c r="D34" s="22" cm="1">
-        <f t="array" ref="D34">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C34)</f>
-        <v>8</v>
-      </c>
-      <c r="E34" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="10">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="C35" s="10">
-        <f t="shared" si="0"/>
-        <v>511</v>
-      </c>
-      <c r="D35" s="22" cm="1">
-        <f t="array" ref="D35">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C35)</f>
-        <v>9</v>
-      </c>
-      <c r="E35" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="10">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="C36" s="10">
-        <f t="shared" si="0"/>
-        <v>1023</v>
-      </c>
-      <c r="D36" s="22" cm="1">
-        <f t="array" ref="D36">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C36)</f>
-        <v>10</v>
-      </c>
-      <c r="E36" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="10">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="C37" s="10">
-        <f t="shared" si="0"/>
-        <v>2047</v>
-      </c>
-      <c r="D37" s="22" cm="1">
-        <f t="array" ref="D37">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C37)</f>
-        <v>11</v>
-      </c>
-      <c r="E37" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="10">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="C38" s="10">
-        <f t="shared" si="0"/>
-        <v>4095</v>
-      </c>
-      <c r="D38" s="22" cm="1">
-        <f t="array" ref="D38">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C38)</f>
-        <v>12</v>
-      </c>
-      <c r="E38" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="10">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="C39" s="10">
-        <f t="shared" si="0"/>
-        <v>8191</v>
-      </c>
-      <c r="D39" s="22" cm="1">
-        <f t="array" ref="D39">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C39)</f>
-        <v>13</v>
-      </c>
-      <c r="E39" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="10">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="C40" s="10">
-        <f t="shared" si="0"/>
-        <v>16383</v>
-      </c>
-      <c r="D40" s="22" cm="1">
-        <f t="array" ref="D40">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C40)</f>
-        <v>14</v>
-      </c>
-      <c r="E40" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="10">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="C41" s="10">
-        <f t="shared" si="0"/>
-        <v>32767</v>
-      </c>
-      <c r="D41" s="22" cm="1">
-        <f t="array" ref="D41">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C41)</f>
-        <v>15</v>
-      </c>
-      <c r="E41" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="10">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="C42" s="10">
-        <f t="shared" si="0"/>
-        <v>65535</v>
-      </c>
-      <c r="D42" s="22" cm="1">
-        <f t="array" ref="D42">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C42)</f>
-        <v>16</v>
-      </c>
-      <c r="E42" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="10">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="C43" s="10">
-        <f t="shared" si="0"/>
-        <v>131071</v>
-      </c>
-      <c r="D43" s="22" cm="1">
-        <f t="array" ref="D43">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C43)</f>
-        <v>17</v>
-      </c>
-      <c r="E43" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="10">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="C44" s="10">
-        <f t="shared" si="0"/>
-        <v>262143</v>
-      </c>
-      <c r="D44" s="22" cm="1">
-        <f t="array" ref="D44">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C44)</f>
-        <v>18</v>
-      </c>
-      <c r="E44" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="10">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="C45" s="10">
-        <f t="shared" si="0"/>
-        <v>524287</v>
-      </c>
-      <c r="D45" s="22" cm="1">
-        <f t="array" ref="D45">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C45)</f>
-        <v>19</v>
-      </c>
-      <c r="E45" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B46" s="10">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="C46" s="10">
-        <f t="shared" si="0"/>
-        <v>1048575</v>
-      </c>
-      <c r="D46" s="22" cm="1">
-        <f t="array" ref="D46">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C46)</f>
-        <v>20</v>
-      </c>
-      <c r="E46" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B47" s="10">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="C47" s="10">
-        <f t="shared" si="0"/>
-        <v>2097151</v>
-      </c>
-      <c r="D47" s="22" cm="1">
-        <f t="array" ref="D47">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C47)</f>
-        <v>21</v>
-      </c>
-      <c r="E47" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="10">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="C48" s="10">
-        <f t="shared" si="0"/>
-        <v>4194303</v>
-      </c>
-      <c r="D48" s="22" cm="1">
-        <f t="array" ref="D48">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C48)</f>
-        <v>22</v>
-      </c>
-      <c r="E48" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B49" s="10">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="C49" s="10">
-        <f t="shared" si="0"/>
-        <v>8388607</v>
-      </c>
-      <c r="D49" s="22" cm="1">
-        <f t="array" ref="D49">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C49)</f>
-        <v>23</v>
-      </c>
-      <c r="E49" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B50" s="10">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="C50" s="10">
-        <f t="shared" si="0"/>
-        <v>16777215</v>
-      </c>
-      <c r="D50" s="22" cm="1">
-        <f t="array" ref="D50">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C50)</f>
-        <v>24</v>
-      </c>
-      <c r="E50" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B51" s="10">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="C51" s="10">
-        <f t="shared" si="0"/>
-        <v>33554431</v>
-      </c>
-      <c r="D51" s="22" cm="1">
-        <f t="array" ref="D51">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C51)</f>
-        <v>25</v>
-      </c>
-      <c r="E51" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B52" s="10">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="C52" s="10">
-        <f t="shared" si="0"/>
-        <v>67108863</v>
-      </c>
-      <c r="D52" s="22" cm="1">
-        <f t="array" ref="D52">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C52)</f>
-        <v>26</v>
-      </c>
-      <c r="E52" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B53" s="10">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="C53" s="10">
-        <f t="shared" si="0"/>
-        <v>134217727</v>
-      </c>
-      <c r="D53" s="22" cm="1">
-        <f t="array" ref="D53">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C53)</f>
-        <v>27</v>
-      </c>
-      <c r="E53" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B54" s="10">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="C54" s="10">
-        <f t="shared" si="0"/>
-        <v>268435455</v>
-      </c>
-      <c r="D54" s="22" cm="1">
-        <f t="array" ref="D54">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C54)</f>
-        <v>28</v>
-      </c>
-      <c r="E54" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B55" s="10">
-        <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="C55" s="10">
-        <f t="shared" si="0"/>
-        <v>536870911</v>
-      </c>
-      <c r="D55" s="22" cm="1">
-        <f t="array" ref="D55">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C55)</f>
-        <v>29</v>
-      </c>
-      <c r="E55" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B56" s="10">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="C56" s="10">
-        <f t="shared" si="0"/>
-        <v>1073741823</v>
-      </c>
-      <c r="D56" s="22" cm="1">
-        <f t="array" ref="D56">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C56)</f>
-        <v>30</v>
-      </c>
-      <c r="E56" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B57" s="10">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="C57" s="10">
-        <f t="shared" si="0"/>
-        <v>2147483647</v>
-      </c>
-      <c r="D57" s="22" cm="1">
-        <f t="array" ref="D57">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C57)</f>
-        <v>31</v>
-      </c>
-      <c r="E57" s="10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B58" s="10">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="C58" s="10">
-        <f t="shared" ref="C58:C76" si="3">2^B58-1</f>
-        <v>4294967295</v>
-      </c>
-      <c r="D58" s="22" cm="1">
-        <f t="array" ref="D58">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C58)</f>
-        <v>32</v>
-      </c>
-      <c r="E58" s="10" t="b">
-        <f t="shared" ref="E58:E76" si="4">D58=B58</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B59" s="10">
-        <f t="shared" ref="B59:B76" si="5">B58+1</f>
-        <v>33</v>
-      </c>
-      <c r="C59" s="10">
-        <f t="shared" si="3"/>
-        <v>8589934591</v>
-      </c>
-      <c r="D59" s="22" cm="1">
-        <f t="array" ref="D59">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C59)</f>
-        <v>33</v>
-      </c>
-      <c r="E59" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B60" s="10">
-        <f t="shared" si="5"/>
-        <v>34</v>
-      </c>
-      <c r="C60" s="10">
-        <f t="shared" si="3"/>
-        <v>17179869183</v>
-      </c>
-      <c r="D60" s="22" cm="1">
-        <f t="array" ref="D60">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C60)</f>
-        <v>34</v>
-      </c>
-      <c r="E60" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B61" s="10">
-        <f t="shared" si="5"/>
-        <v>35</v>
-      </c>
-      <c r="C61" s="10">
-        <f t="shared" si="3"/>
-        <v>34359738367</v>
-      </c>
-      <c r="D61" s="22" cm="1">
-        <f t="array" ref="D61">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C61)</f>
-        <v>35</v>
-      </c>
-      <c r="E61" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B62" s="10">
-        <f t="shared" si="5"/>
-        <v>36</v>
-      </c>
-      <c r="C62" s="10">
-        <f t="shared" si="3"/>
-        <v>68719476735</v>
-      </c>
-      <c r="D62" s="22" cm="1">
-        <f t="array" ref="D62">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C62)</f>
-        <v>36</v>
-      </c>
-      <c r="E62" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B63" s="10">
-        <f t="shared" si="5"/>
-        <v>37</v>
-      </c>
-      <c r="C63" s="10">
-        <f t="shared" si="3"/>
-        <v>137438953471</v>
-      </c>
-      <c r="D63" s="22" cm="1">
-        <f t="array" ref="D63">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C63)</f>
-        <v>37</v>
-      </c>
-      <c r="E63" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B64" s="10">
-        <f t="shared" si="5"/>
-        <v>38</v>
-      </c>
-      <c r="C64" s="10">
-        <f t="shared" si="3"/>
-        <v>274877906943</v>
-      </c>
-      <c r="D64" s="22" cm="1">
-        <f t="array" ref="D64">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C64)</f>
-        <v>38</v>
-      </c>
-      <c r="E64" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B65" s="10">
-        <f t="shared" si="5"/>
-        <v>39</v>
-      </c>
-      <c r="C65" s="10">
-        <f t="shared" si="3"/>
-        <v>549755813887</v>
-      </c>
-      <c r="D65" s="22" cm="1">
-        <f t="array" ref="D65">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C65)</f>
-        <v>39</v>
-      </c>
-      <c r="E65" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B66" s="10">
-        <f t="shared" si="5"/>
-        <v>40</v>
-      </c>
-      <c r="C66" s="10">
-        <f t="shared" si="3"/>
-        <v>1099511627775</v>
-      </c>
-      <c r="D66" s="22" cm="1">
-        <f t="array" ref="D66">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C66)</f>
-        <v>40</v>
-      </c>
-      <c r="E66" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B67" s="10">
-        <f t="shared" si="5"/>
-        <v>41</v>
-      </c>
-      <c r="C67" s="10">
-        <f t="shared" si="3"/>
-        <v>2199023255551</v>
-      </c>
-      <c r="D67" s="22" cm="1">
-        <f t="array" ref="D67">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C67)</f>
-        <v>41</v>
-      </c>
-      <c r="E67" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B68" s="10">
-        <f t="shared" si="5"/>
-        <v>42</v>
-      </c>
-      <c r="C68" s="10">
-        <f t="shared" si="3"/>
-        <v>4398046511103</v>
-      </c>
-      <c r="D68" s="22" cm="1">
-        <f t="array" ref="D68">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C68)</f>
-        <v>42</v>
-      </c>
-      <c r="E68" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B69" s="10">
-        <f t="shared" si="5"/>
-        <v>43</v>
-      </c>
-      <c r="C69" s="10">
-        <f t="shared" si="3"/>
-        <v>8796093022207</v>
-      </c>
-      <c r="D69" s="22" cm="1">
-        <f t="array" ref="D69">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C69)</f>
-        <v>43</v>
-      </c>
-      <c r="E69" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B70" s="10">
-        <f t="shared" si="5"/>
-        <v>44</v>
-      </c>
-      <c r="C70" s="10">
-        <f t="shared" si="3"/>
-        <v>17592186044415</v>
-      </c>
-      <c r="D70" s="22" cm="1">
-        <f t="array" ref="D70">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C70)</f>
-        <v>44</v>
-      </c>
-      <c r="E70" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B71" s="1">
-        <f t="shared" si="5"/>
-        <v>45</v>
-      </c>
-      <c r="C71" s="1">
-        <f t="shared" si="3"/>
-        <v>35184372088831</v>
-      </c>
-      <c r="D71" s="27" cm="1">
-        <f t="array" ref="D71">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C71)</f>
-        <v>46</v>
-      </c>
-      <c r="E71" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B72" s="10">
-        <f t="shared" si="5"/>
-        <v>46</v>
-      </c>
-      <c r="C72" s="10">
-        <f t="shared" si="3"/>
-        <v>70368744177663</v>
-      </c>
-      <c r="D72" s="22" cm="1">
-        <f t="array" ref="D72">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C72)</f>
-        <v>47</v>
-      </c>
-      <c r="E72" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B73" s="10">
-        <f t="shared" si="5"/>
-        <v>47</v>
-      </c>
-      <c r="C73" s="10">
-        <f t="shared" si="3"/>
-        <v>140737488355327</v>
-      </c>
-      <c r="D73" s="22" cm="1">
-        <f t="array" ref="D73">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C73)</f>
-        <v>48</v>
-      </c>
-      <c r="E73" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B74" s="10">
-        <f t="shared" si="5"/>
-        <v>48</v>
-      </c>
-      <c r="C74" s="10">
-        <f t="shared" si="3"/>
-        <v>281474976710655</v>
-      </c>
-      <c r="D74" s="22" cm="1">
-        <f t="array" ref="D74">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C74)</f>
-        <v>49</v>
-      </c>
-      <c r="E74" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B75" s="10">
-        <f t="shared" si="5"/>
-        <v>49</v>
-      </c>
-      <c r="C75" s="10">
-        <f t="shared" si="3"/>
-        <v>562949953421311</v>
-      </c>
-      <c r="D75" s="22" cm="1">
-        <f t="array" ref="D75">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C75)</f>
-        <v>50</v>
-      </c>
-      <c r="E75" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B76" s="10">
-        <f t="shared" si="5"/>
-        <v>50</v>
-      </c>
-      <c r="C76" s="10">
-        <f t="shared" si="3"/>
-        <v>1125899906842623</v>
-      </c>
-      <c r="D76" s="22" cm="1">
-        <f t="array" ref="D76">_xlfn.LAMBDA(_xlpm.I, INT(IF(_xlpm.I, LOG(ABS(_xlpm.I), 2) + 1)))(C76)</f>
-        <v>51</v>
-      </c>
-      <c r="E76" s="10" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -4354,22 +3281,22 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="15" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="21" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -4403,7 +3330,7 @@
         <v>False</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
@@ -4416,7 +3343,7 @@
         <v>True</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
@@ -4450,7 +3377,7 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="10" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
@@ -4616,7 +3543,7 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
@@ -4624,17 +3551,17 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
-        <v>491</v>
+        <v>481</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="21" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -4645,7 +3572,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E10" s="1" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -4653,10 +3580,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -4668,7 +3595,7 @@
         <v>-123</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
@@ -4680,7 +3607,7 @@
         <v>-1</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
@@ -4722,7 +3649,7 @@
         <v>123.456</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
@@ -4742,7 +3669,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E22" s="22" t="s">
         <v>97</v>
@@ -4796,7 +3723,7 @@
         <v>0b1111111111</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
@@ -4867,7 +3794,7 @@
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E37" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
@@ -4875,10 +3802,10 @@
         <v>23</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
@@ -4890,7 +3817,7 @@
         <v>9</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
@@ -4902,7 +3829,7 @@
         <v>8</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
@@ -4966,7 +3893,7 @@
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C48" s="22"/>
       <c r="E48" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -4974,10 +3901,10 @@
         <v>23</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
@@ -4989,7 +3916,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
@@ -5059,10 +3986,10 @@
         <v>23</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
@@ -5074,12 +4001,12 @@
         <v>0</v>
       </c>
       <c r="E64" s="22" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E65" s="22" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
@@ -5098,7 +4025,7 @@
         <v>23</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E69" s="22" t="s">
         <v>103</v>
@@ -5152,7 +4079,7 @@
         <v>0xFFFFFFFFFF</v>
       </c>
       <c r="E75" s="22" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
@@ -5236,7 +4163,7 @@
         <v>23</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E85" s="22" t="s">
         <v>111</v>
@@ -5290,7 +4217,7 @@
         <v>0x7777777777</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.2">
@@ -5358,18 +4285,18 @@
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E100" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="101" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B101" s="9" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.2">
@@ -5424,7 +4351,7 @@
         <v>0</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.2">
@@ -5448,7 +4375,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="E113" s="10" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.2">
@@ -5460,23 +4387,23 @@
         <v>#VALUE!</v>
       </c>
       <c r="E114" s="10" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
     </row>
     <row r="117" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E117" s="1" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
     </row>
     <row r="118" spans="2:5" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B118" s="9" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C118" s="25" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="120" spans="2:5" x14ac:dyDescent="0.2">
@@ -5546,7 +4473,7 @@
         <v>-0.4</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.2">
@@ -5564,18 +4491,18 @@
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E136" s="1" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="137" spans="2:5" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B137" s="9" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C137" s="25" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="138" spans="2:5" x14ac:dyDescent="0.2">
@@ -5640,7 +4567,7 @@
         <v>0.5</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.2">
@@ -5661,7 +4588,7 @@
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E152" s="1" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
     </row>
     <row r="153" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -5669,10 +4596,10 @@
         <v>40</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.2">
@@ -5686,12 +4613,12 @@
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E157" s="1" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
     </row>
     <row r="158" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="E158" s="2" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
     </row>
     <row r="159" spans="2:5" x14ac:dyDescent="0.2">
@@ -5699,7 +4626,7 @@
         <v>40</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
     </row>
     <row r="160" spans="2:5" x14ac:dyDescent="0.2">
@@ -5713,17 +4640,17 @@
     </row>
     <row r="163" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E163" s="1" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
     </row>
     <row r="164" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E164" s="10" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
     </row>
     <row r="165" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E165" s="10" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -5749,22 +4676,22 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
-        <v>492</v>
+        <v>482</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -5776,13 +4703,13 @@
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="8"/>
       <c r="E10" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="8"/>
       <c r="E11" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
@@ -5798,7 +4725,7 @@
         <v>84</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
@@ -5810,7 +4737,7 @@
         <v>-123.0</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -5822,7 +4749,7 @@
         <v>-1.23</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
@@ -5927,7 +4854,7 @@
         <v>42</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -5939,7 +4866,7 @@
         <v>-1</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -5951,7 +4878,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
@@ -5976,7 +4903,7 @@
         <v>87</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
@@ -5995,7 +4922,7 @@
     </row>
     <row r="45" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="E45" s="2" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
@@ -6038,17 +4965,17 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
@@ -6062,7 +4989,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E10" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -6070,7 +4997,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>37</v>
@@ -6085,19 +5012,19 @@
         <v>0</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="21" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C13" s="16" t="b" cm="1">
         <f t="array" ref="C13">str.bool(B13)</f>
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
@@ -6106,7 +5033,7 @@
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="8"/>
       <c r="E16" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -6114,7 +5041,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E17" s="22" t="s">
         <v>37</v>
@@ -6129,12 +5056,12 @@
         <v>0</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="21" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C19" s="16" t="b" cm="1">
         <f t="array" ref="C19">str.bool(B19)</f>
@@ -6148,18 +5075,18 @@
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="E22" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="9" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
@@ -6168,19 +5095,19 @@
     </row>
     <row r="25" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B25" s="21" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C25" s="26" t="b" cm="1">
         <f t="array" ref="C25">str.endswith(B25,B26)</f>
         <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="21" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C26" s="26"/>
       <c r="E26" s="2"/>
@@ -6192,19 +5119,19 @@
     </row>
     <row r="28" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B28" s="21" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C28" s="26" t="b" cm="1">
         <f t="array" ref="C28">str.endswith(B28,B29)</f>
         <v>0</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="21" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="E29" s="2"/>
     </row>
@@ -6215,14 +5142,14 @@
     </row>
     <row r="31" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B31" s="21" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C31" s="26" t="b" cm="1">
         <f t="array" ref="C31">str.endswith(B31,B32)</f>
         <v>1</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
@@ -6230,7 +5157,7 @@
         <v>29</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
@@ -6246,7 +5173,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
@@ -6254,7 +5181,7 @@
         <v>29</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
@@ -6276,12 +5203,12 @@
         <v>74</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>167</v>
+        <v>508</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E40" s="3" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
@@ -6293,7 +5220,7 @@
         <v/>
       </c>
       <c r="E41" s="3" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
@@ -6353,36 +5280,36 @@
         <v>ab'cd</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="21" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C50" s="16" t="str" cm="1">
         <f t="array" ref="C50">str.eval(B50)</f>
         <v>bcde</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="21" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C51" s="16" t="e" cm="1">
         <f t="array" ref="C51">str.eval(B51)</f>
         <v>#VALUE!</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E54" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="2:5" ht="176" customHeight="1" x14ac:dyDescent="0.2">
@@ -6390,10 +5317,10 @@
         <v>27</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
@@ -6401,7 +5328,7 @@
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C57" s="16" cm="1">
         <f t="array" ref="C57">str.int(B57)</f>
@@ -6415,7 +5342,7 @@
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C58" s="16" cm="1">
         <f t="array" ref="C58">str.int(B58)</f>
@@ -6429,7 +5356,7 @@
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C59" s="16" cm="1">
         <f t="array" ref="C59">str.int(B59)</f>
@@ -6443,7 +5370,7 @@
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C60" s="16" cm="1">
         <f t="array" ref="C60">str.int(B60)</f>
@@ -6461,26 +5388,26 @@
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" s="21" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C62" s="16" t="e" cm="1">
         <f t="array" ref="C62">str.int(B62)</f>
         <v>#NUM!</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" s="21" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C63" s="16" t="e" cm="1">
         <f t="array" ref="C63">str.int(B63)</f>
         <v>#NUM!</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
@@ -6489,34 +5416,34 @@
         <v>#NUM!</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E65" s="10" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="E66" s="10" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E67" s="3" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E70" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E71" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.2">
@@ -6524,12 +5451,12 @@
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E74" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="2:5" ht="224" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E75" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
@@ -6540,12 +5467,12 @@
         <v>27</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B79" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C79" s="16" cm="1">
         <f t="array" ref="C79">str.int_base_2(B79)</f>
@@ -6555,7 +5482,7 @@
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B80" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C80" s="16" cm="1">
         <f t="array" ref="C80">str.int_base_2(B80)</f>
@@ -6569,19 +5496,19 @@
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B82" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C82" s="16" cm="1">
         <f t="array" ref="C82">str.int_base_2(B82)</f>
         <v>15</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B83" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C83" s="16" cm="1">
         <f t="array" ref="C83">str.int_base_2(B83)</f>
@@ -6591,7 +5518,7 @@
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B84" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C84" s="16" cm="1">
         <f t="array" ref="C84">str.int_base_2(B84)</f>
@@ -6601,7 +5528,7 @@
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B85" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C85" s="16" cm="1">
         <f t="array" ref="C85">str.int_base_2(B85)</f>
@@ -6615,7 +5542,7 @@
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B87" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E87" s="1"/>
     </row>
@@ -6629,7 +5556,7 @@
         <v>512</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.2">
@@ -6638,14 +5565,14 @@
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B90" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C90" s="16" t="e" cm="1">
         <f t="array" ref="C90">str.int_base_2(B90)</f>
         <v>#NUM!</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.2">
@@ -6654,50 +5581,50 @@
         <v>#NUM!</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E94" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E95" s="10" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E97" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E98" s="10" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E100" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E101" s="10" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B103" s="15" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="104" spans="2:5" ht="136" x14ac:dyDescent="0.2">
       <c r="E104" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.2">
@@ -6708,18 +5635,18 @@
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B107" s="15" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="C107" s="10"/>
       <c r="E107" s="1" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B108" s="10"/>
       <c r="C108" s="10"/>
       <c r="E108" s="22" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.2">
@@ -6734,12 +5661,12 @@
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E111" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E112" s="22" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.2">
@@ -6747,7 +5674,7 @@
         <v>28</v>
       </c>
       <c r="C113" s="16" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E113" s="22"/>
     </row>
@@ -6774,7 +5701,7 @@
     </row>
     <row r="118" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B118" s="21" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="C118" s="16" cm="1">
         <f t="array" ref="C118">str.ord(B118)</f>
@@ -6789,10 +5716,10 @@
     </row>
     <row r="121" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B121" s="15" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="122" spans="2:5" x14ac:dyDescent="0.2">
@@ -6805,12 +5732,12 @@
     </row>
     <row r="124" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E124" s="4" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="125" spans="2:5" ht="192" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E125" s="2" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
     </row>
     <row r="126" spans="2:5" x14ac:dyDescent="0.2">
@@ -6818,7 +5745,7 @@
     </row>
     <row r="127" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B127" s="22" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
     </row>
     <row r="128" spans="2:5" x14ac:dyDescent="0.2">
@@ -6856,7 +5783,7 @@
     </row>
     <row r="135" spans="2:5" ht="192" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E135" s="2" t="s">
-        <v>170</v>
+        <v>509</v>
       </c>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.2">
@@ -6910,7 +5837,7 @@
         <v>'ab\'cd'</v>
       </c>
       <c r="E141" s="10" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.2">
@@ -6939,12 +5866,12 @@
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E146" s="4" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E147" s="22" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.2">
@@ -6952,12 +5879,12 @@
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E149" s="4" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
     </row>
     <row r="150" spans="2:5" ht="208" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E150" s="2" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
     </row>
     <row r="151" spans="2:5" x14ac:dyDescent="0.2">
@@ -6965,7 +5892,7 @@
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B152" s="22" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.2">
@@ -6996,12 +5923,12 @@
     </row>
     <row r="159" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E159" s="4" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="160" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E160" s="22" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="161" spans="5:5" x14ac:dyDescent="0.2">
@@ -7009,17 +5936,17 @@
     </row>
     <row r="162" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E162" s="4" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="163" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E163" s="22" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="169" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E169" s="10" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -7030,7 +5957,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9AEAAA-FB17-324F-AABB-3625663F090B}">
-  <dimension ref="B3:E102"/>
+  <dimension ref="B3:E113"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
@@ -7046,17 +5973,17 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
-        <v>490</v>
+        <v>480</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
@@ -7172,7 +6099,7 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="21" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E29" s="22"/>
     </row>
@@ -7245,7 +6172,7 @@
       <c r="C43" s="13"/>
       <c r="D43" s="3"/>
       <c r="E43" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -7253,11 +6180,11 @@
         <v>54</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
@@ -7268,7 +6195,7 @@
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C46" s="13" t="e" cm="1">
         <f t="array" ref="C46">list.bool(B46)</f>
@@ -7276,7 +6203,7 @@
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
@@ -7287,7 +6214,7 @@
       <c r="C47" s="13"/>
       <c r="D47" s="3"/>
       <c r="E47" s="10" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
@@ -7316,7 +6243,7 @@
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C51" s="13"/>
       <c r="D51" s="3"/>
@@ -7329,14 +6256,14 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="18" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
@@ -7358,10 +6285,10 @@
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" s="18" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -7388,7 +6315,7 @@
         <v>120</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -7422,7 +6349,7 @@
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" s="11"/>
       <c r="C64" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -7448,7 +6375,7 @@
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E68" s="4" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="69" spans="2:5" ht="80" customHeight="1" x14ac:dyDescent="0.2">
@@ -7456,10 +6383,10 @@
         <v>54</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
@@ -7469,7 +6396,7 @@
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" s="18" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C71" s="13"/>
       <c r="E71" s="3"/>
@@ -7514,14 +6441,14 @@
       <c r="B76" s="11"/>
       <c r="C76" s="13"/>
       <c r="E76" s="4" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
     </row>
     <row r="77" spans="2:5" ht="85" x14ac:dyDescent="0.2">
       <c r="B77" s="11"/>
       <c r="C77" s="13"/>
       <c r="E77" s="6" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.2">
@@ -7541,15 +6468,15 @@
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E81" s="4" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="82" spans="2:5" ht="51" x14ac:dyDescent="0.2">
       <c r="C82" s="32" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="83" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -7605,12 +6532,12 @@
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E91" s="4" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E92" s="3" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.2">
@@ -7632,7 +6559,7 @@
       <c r="C96" s="13"/>
       <c r="D96" s="3"/>
       <c r="E96" s="6" t="s">
-        <v>128</v>
+        <v>510</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.2">
@@ -7640,7 +6567,7 @@
         <v>54</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D97" s="3"/>
       <c r="E97" s="5"/>
@@ -7668,6 +6595,67 @@
     <row r="102" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B102" s="15">
         <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B104" s="21" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B105" s="15" t="str" cm="1">
+        <f t="array" ref="B105:B107">CHOOSE({1;2;3},"aa","bb","cc")</f>
+        <v>aa</v>
+      </c>
+      <c r="C105" s="13" t="str" cm="1">
+        <f t="array" ref="C105">list.repr(_xlfn.ANCHORARRAY(B105))</f>
+        <v>[aa, bb, cc]</v>
+      </c>
+      <c r="E105" s="10" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B106" s="15" t="str">
+        <v>bb</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B107" s="15" t="str">
+        <v>cc</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C109" s="16" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B110" s="21" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B111" s="15" t="str" cm="1">
+        <f t="array" ref="B111:B113">CHOOSE({1;2;3},"aa","bb","cc")</f>
+        <v>aa</v>
+      </c>
+      <c r="C111" s="13" t="e" cm="1">
+        <f t="array" ref="C111">str.repr(_xlfn.ANCHORARRAY(B111))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E111" s="10" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B112" s="15" t="str">
+        <v>bb</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B113" s="15" t="str">
+        <v>cc</v>
       </c>
     </row>
   </sheetData>
@@ -7693,22 +6681,22 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
-        <v>502</v>
+        <v>492</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="15" t="s">
-        <v>501</v>
+        <v>491</v>
       </c>
       <c r="C7" s="19"/>
     </row>
@@ -7721,13 +6709,13 @@
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C10" s="19"/>
       <c r="E10" s="4" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C11" s="19"/>
       <c r="E11" s="14" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -7741,13 +6729,13 @@
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C14" s="19"/>
       <c r="E14" s="4" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="19"/>
       <c r="E15" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
@@ -7761,12 +6749,12 @@
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C18" s="19"/>
       <c r="E18" s="4" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="102" x14ac:dyDescent="0.2">
       <c r="E19" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
@@ -7774,7 +6762,7 @@
         <v>45</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E20" s="6"/>
     </row>
@@ -7790,7 +6778,7 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C22" s="16" t="b" cm="1">
         <f t="array" ref="C22">_any(B22)</f>
@@ -7806,7 +6794,7 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E25" s="4" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
@@ -7817,7 +6805,7 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E28" s="4" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
@@ -7833,7 +6821,7 @@
     </row>
     <row r="32" spans="2:5" ht="119" x14ac:dyDescent="0.2">
       <c r="E32" s="6" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
@@ -7995,14 +6983,14 @@
       <c r="B54" s="18"/>
       <c r="C54" s="13"/>
       <c r="E54" s="4" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="18"/>
       <c r="C55" s="13"/>
       <c r="E55" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
@@ -8013,7 +7001,7 @@
       <c r="B57" s="18"/>
       <c r="C57" s="13"/>
       <c r="E57" s="4" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
@@ -8025,7 +7013,7 @@
       <c r="B59" s="18"/>
       <c r="C59" s="13"/>
       <c r="E59" s="4" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
@@ -8036,7 +7024,7 @@
       <c r="B61" s="18"/>
       <c r="C61" s="13"/>
       <c r="E61" s="4" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
@@ -8048,14 +7036,14 @@
       <c r="B63" s="18"/>
       <c r="C63" s="13"/>
       <c r="E63" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" s="18"/>
       <c r="C64" s="13"/>
       <c r="E64" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
@@ -8067,7 +7055,7 @@
       <c r="B66" s="18"/>
       <c r="C66" s="13"/>
       <c r="E66" s="4" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
@@ -8078,14 +7066,14 @@
       <c r="B68" s="18"/>
       <c r="C68" s="13"/>
       <c r="E68" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="2:5" ht="85" x14ac:dyDescent="0.2">
       <c r="B69" s="18"/>
       <c r="C69" s="13"/>
       <c r="E69" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
@@ -8097,7 +7085,7 @@
       <c r="B71" s="18"/>
       <c r="C71" s="13"/>
       <c r="E71" s="4" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.2">
@@ -8109,7 +7097,7 @@
       <c r="B73" s="18"/>
       <c r="C73" s="13"/>
       <c r="E73" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.2">
@@ -8121,7 +7109,7 @@
       <c r="B75" s="18"/>
       <c r="C75" s="13"/>
       <c r="E75" s="4" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
@@ -8133,7 +7121,7 @@
       <c r="B77" s="18"/>
       <c r="C77" s="13"/>
       <c r="E77" s="4" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.2">
@@ -8145,7 +7133,7 @@
       <c r="B79" s="18"/>
       <c r="C79" s="13"/>
       <c r="E79" s="4" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.2">
@@ -8157,7 +7145,7 @@
       <c r="B81" s="18"/>
       <c r="C81" s="13"/>
       <c r="E81" s="4" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.2">
@@ -8169,7 +7157,7 @@
       <c r="B83" s="18"/>
       <c r="C83" s="13"/>
       <c r="E83" s="4" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.2">
@@ -8181,7 +7169,7 @@
       <c r="B85" s="18"/>
       <c r="C85" s="13"/>
       <c r="E85" s="4" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.2">
@@ -8193,7 +7181,7 @@
       <c r="B87" s="18"/>
       <c r="C87" s="13"/>
       <c r="E87" s="4" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.2">
@@ -8205,21 +7193,21 @@
       <c r="B89" s="18"/>
       <c r="C89" s="13"/>
       <c r="E89" s="4" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B90" s="18"/>
       <c r="C90" s="13"/>
       <c r="E90" s="4" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B91" s="18"/>
       <c r="C91" s="13"/>
       <c r="E91" s="4" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.2">
@@ -8240,7 +7228,7 @@
       <c r="C94" s="13"/>
       <c r="D94" s="3"/>
       <c r="E94" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.2">
@@ -8291,7 +7279,7 @@
       </c>
       <c r="D99" s="3"/>
       <c r="E99" s="5" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.2">
@@ -8365,12 +7353,12 @@
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E109" s="4" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E110" s="22" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.2">
@@ -8378,12 +7366,12 @@
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E112" s="4" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="113" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E113" s="22" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="114" spans="5:5" x14ac:dyDescent="0.2">
@@ -8391,12 +7379,12 @@
     </row>
     <row r="115" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E115" s="4" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="116" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E116" s="22" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="117" spans="5:5" x14ac:dyDescent="0.2">
@@ -8404,17 +7392,17 @@
     </row>
     <row r="118" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E118" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="119" spans="5:5" ht="102" x14ac:dyDescent="0.2">
       <c r="E119" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="121" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E121" s="4" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -8478,34 +7466,34 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="10" t="s">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>510</v>
+        <v>500</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>512</v>
+        <v>502</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.2">
@@ -8566,26 +7554,26 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" s="10" t="s">
-        <v>504</v>
+        <v>494</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>503</v>
+        <v>493</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" s="10" t="s">
-        <v>505</v>
+        <v>495</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>506</v>
+        <v>496</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" s="10" t="s">
-        <v>507</v>
+        <v>497</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>508</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -8603,7 +7591,7 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
@@ -8611,7 +7599,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
@@ -8619,109 +7607,109 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="10" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="10" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="10" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
@@ -8732,7 +7720,7 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
@@ -8741,23 +7729,23 @@
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C24" s="9"/>
       <c r="D24" s="9" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="E25" s="33"/>
       <c r="F25" s="33"/>
       <c r="G25" s="9" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
@@ -8778,11 +7766,11 @@
       </c>
       <c r="D27" s="33"/>
       <c r="E27" s="34" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="F27" s="33"/>
       <c r="G27" s="33" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
@@ -8796,11 +7784,11 @@
       </c>
       <c r="D28" s="33"/>
       <c r="E28" s="34" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="F28" s="33"/>
       <c r="G28" s="33" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
@@ -8813,7 +7801,7 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" s="34" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
@@ -8832,11 +7820,11 @@
       </c>
       <c r="D31" s="33"/>
       <c r="E31" s="34" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="F31" s="33"/>
       <c r="G31" s="33" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
@@ -8853,7 +7841,7 @@
       </c>
       <c r="C33" s="33"/>
       <c r="D33" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E33" s="34"/>
       <c r="F33" s="33"/>
@@ -8873,11 +7861,11 @@
         <v>64</v>
       </c>
       <c r="E34" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="F34" s="33"/>
       <c r="G34" s="33" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
@@ -8890,7 +7878,7 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" s="34" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="C36" s="33">
         <f>TYPE(B36)</f>
@@ -8898,11 +7886,11 @@
       </c>
       <c r="D36" s="33"/>
       <c r="E36" s="33" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="F36" s="33"/>
       <c r="G36" s="33" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
@@ -8923,11 +7911,11 @@
       </c>
       <c r="D38" s="33"/>
       <c r="E38" s="33" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="F38" s="33"/>
       <c r="G38" s="33" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
@@ -8952,7 +7940,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="33" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F40" s="33"/>
       <c r="G40" s="33"/>
@@ -8971,7 +7959,7 @@
         <v>2</v>
       </c>
       <c r="E41" s="33" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F41" s="33"/>
       <c r="G41" s="33"/>
@@ -8989,7 +7977,7 @@
         <v>3</v>
       </c>
       <c r="E42" s="33" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F42" s="33"/>
       <c r="G42" s="33"/>
@@ -9008,7 +7996,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="33" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F43" s="33"/>
       <c r="G43" s="33"/>
@@ -9027,7 +8015,7 @@
         <v>5</v>
       </c>
       <c r="E44" s="33" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F44" s="33"/>
       <c r="G44" s="33"/>
@@ -9046,7 +8034,7 @@
         <v>6</v>
       </c>
       <c r="E45" s="33" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F45" s="33"/>
       <c r="G45" s="33"/>
@@ -9065,7 +8053,7 @@
         <v>7</v>
       </c>
       <c r="E46" s="33" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F46" s="33"/>
       <c r="G46" s="33"/>
@@ -9094,7 +8082,7 @@
         <v>9</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F48" s="33"/>
       <c r="G48" s="33"/>
@@ -9143,7 +8131,7 @@
         <v>13</v>
       </c>
       <c r="E52" s="33" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F52" s="33"/>
       <c r="G52" s="33"/>
@@ -9162,14 +8150,14 @@
         <v>14</v>
       </c>
       <c r="E53" s="33" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F53" s="33"/>
       <c r="G53" s="33"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B54" s="34" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="C54" s="33">
         <v>16</v>
@@ -9179,7 +8167,7 @@
         <v>#N/A</v>
       </c>
       <c r="E54" s="33" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F54" s="33"/>
       <c r="G54" s="33"/>
@@ -9199,11 +8187,11 @@
       </c>
       <c r="D56" s="33"/>
       <c r="E56" s="33" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F56" s="33"/>
       <c r="G56" s="33" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -9228,7 +8216,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -9258,7 +8246,7 @@
         <v>3</v>
       </c>
       <c r="B65" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -9267,7 +8255,7 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -9285,7 +8273,7 @@
         <v>6</v>
       </c>
       <c r="B68" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -9294,7 +8282,7 @@
         <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -9303,7 +8291,7 @@
         <v>8</v>
       </c>
       <c r="B70" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -9312,7 +8300,7 @@
         <v>9</v>
       </c>
       <c r="B71" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -9321,7 +8309,7 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -9330,7 +8318,7 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -9339,7 +8327,7 @@
         <v>12</v>
       </c>
       <c r="B74" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Column H to Sheet Etc
</commit_message>
<xml_diff>
--- a/like-py.xlsx
+++ b/like-py.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plavarre/Public/like-py-xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF32B10-197E-7C4D-8095-4D8AFE8C7F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E18C194-E6B2-744F-9689-966A858DFFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-7900" yWindow="-22000" windowWidth="34040" windowHeight="18000" xr2:uid="{995B5C66-FA72-074C-87BA-100299560140}"/>
   </bookViews>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="579">
   <si>
     <t>bit</t>
   </si>
@@ -2304,6 +2304,9 @@
   </si>
   <si>
     <t>def random.sample(items)</t>
+  </si>
+  <si>
+    <t>Excel Source of Error Instance</t>
   </si>
 </sst>
 </file>
@@ -2411,7 +2414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -2514,6 +2517,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3498,7 +3502,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355B7662-A6AF-4E4B-A8A9-10FF81599954}">
-  <dimension ref="A3:G80"/>
+  <dimension ref="A3:H80"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
@@ -3507,26 +3511,26 @@
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
         <v>258</v>
       </c>
@@ -3541,8 +3545,11 @@
       <c r="G9" s="9" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="33"/>
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
@@ -3550,7 +3557,7 @@
       <c r="F10" s="33"/>
       <c r="G10" s="33"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="33">
         <v>0</v>
       </c>
@@ -3567,7 +3574,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="33">
         <f>1.00000001</f>
         <v>1.0000000099999999</v>
@@ -3585,7 +3592,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="33"/>
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
@@ -3593,7 +3600,7 @@
       <c r="F13" s="33"/>
       <c r="G13" s="33"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="34" t="s">
         <v>279</v>
       </c>
@@ -3603,7 +3610,7 @@
       <c r="F14" s="33"/>
       <c r="G14" s="33"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="33">
         <f>1.000000001</f>
         <v>1.0000000010000001</v>
@@ -3621,7 +3628,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="33"/>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>

</xml_diff>